<commit_message>
doc update and minor bug fixes
</commit_message>
<xml_diff>
--- a/fivecentplots/doc/keywords.xlsx
+++ b/fivecentplots/doc/keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\fivecentplots\fivecentplots\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3DEC275-1FAB-4328-9A3F-009A4D58C4AD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{26DAD7AC-DA79-4C8A-9E4E-7C208FFDF85B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="671" firstSheet="3" activeTab="7" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory" sheetId="11" r:id="rId1"/>
@@ -18,11 +18,14 @@
     <sheet name="Figure" sheetId="5" r:id="rId3"/>
     <sheet name="Axes" sheetId="3" r:id="rId4"/>
     <sheet name="Label" sheetId="6" r:id="rId5"/>
-    <sheet name="Data" sheetId="4" r:id="rId6"/>
-    <sheet name="Box" sheetId="7" r:id="rId7"/>
-    <sheet name="BoxDivider" sheetId="8" r:id="rId8"/>
-    <sheet name="BoxStat" sheetId="9" r:id="rId9"/>
-    <sheet name="BoxRange" sheetId="10" r:id="rId10"/>
+    <sheet name="Ticks" sheetId="13" r:id="rId6"/>
+    <sheet name="Markers" sheetId="14" r:id="rId7"/>
+    <sheet name="Lines" sheetId="4" r:id="rId8"/>
+    <sheet name="Fit" sheetId="15" r:id="rId9"/>
+    <sheet name="Box" sheetId="7" r:id="rId10"/>
+    <sheet name="BoxDivider" sheetId="8" r:id="rId11"/>
+    <sheet name="BoxStat" sheetId="9" r:id="rId12"/>
+    <sheet name="BoxRange" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="214">
   <si>
     <t>Keyword</t>
   </si>
@@ -129,27 +132,6 @@
     <t>ax_scale</t>
   </si>
   <si>
-    <t>share_x</t>
-  </si>
-  <si>
-    <t>share_y</t>
-  </si>
-  <si>
-    <t>share_z</t>
-  </si>
-  <si>
-    <t>share_x2</t>
-  </si>
-  <si>
-    <t>share_y2</t>
-  </si>
-  <si>
-    <t>share_col</t>
-  </si>
-  <si>
-    <t>share_row</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -243,12 +225,6 @@
     <t>dots per inch</t>
   </si>
   <si>
-    <t>twin_x</t>
-  </si>
-  <si>
-    <t>twin_y</t>
-  </si>
-  <si>
     <t>Data Type</t>
   </si>
   <si>
@@ -300,27 +276,6 @@
     <t>calculated automatically</t>
   </si>
   <si>
-    <t>enable/disable primary x-axis range sharing across all subplots</t>
-  </si>
-  <si>
-    <t>enable/disable primary y-axis range sharing across all subplots</t>
-  </si>
-  <si>
-    <t>enable/disable primary z-axis range sharing across all subplots</t>
-  </si>
-  <si>
-    <t>enable/disable secondary x-axis range sharing across all subplots</t>
-  </si>
-  <si>
-    <t>enable/disable secondary y-axis range sharing across all subplots</t>
-  </si>
-  <si>
-    <t>enable/disable axis range sharing for all subplots in a row of subplots</t>
-  </si>
-  <si>
-    <t>enable/disable axis range sharing for all subplots in a column of subplots</t>
-  </si>
-  <si>
     <t>enable/disable a secondary y-axis (x-axis is "twinned" or duplicated across two y-axes)</t>
   </si>
   <si>
@@ -465,22 +420,265 @@
     <t>all except boxplot</t>
   </si>
   <si>
-    <t>always</t>
-  </si>
-  <si>
-    <t>ax_limit_padding</t>
-  </si>
-  <si>
-    <t>conf_int</t>
-  </si>
-  <si>
     <t>fit</t>
   </si>
   <si>
     <t>all except histogram</t>
   </si>
   <si>
-    <t>contour and heatmap</t>
+    <t>always (**note:** ``df`` can also be specified as the first function argument withouth the keyword name of ``df==``)</t>
+  </si>
+  <si>
+    <t>only for contour and heatmap</t>
+  </si>
+  <si>
+    <t>ax_size</t>
+  </si>
+  <si>
+    <t>:hh:`share_x`</t>
+  </si>
+  <si>
+    <t>:hh:`share_y`</t>
+  </si>
+  <si>
+    <t>:hh:`share_z`</t>
+  </si>
+  <si>
+    <t>:hh:`share_x2`</t>
+  </si>
+  <si>
+    <t>:hh:`share_y2`</t>
+  </si>
+  <si>
+    <t>:hh:`share_col`</t>
+  </si>
+  <si>
+    <t>:hh:`share_row`</t>
+  </si>
+  <si>
+    <t>:hh:`twin_x`</t>
+  </si>
+  <si>
+    <t>:hh:`twin_y`</t>
+  </si>
+  <si>
+    <t>:hh:`spines`</t>
+  </si>
+  <si>
+    <t>:hh:`spine_bottom`</t>
+  </si>
+  <si>
+    <t>:hh:`spine_left`</t>
+  </si>
+  <si>
+    <t>:hh:`spine_right`</t>
+  </si>
+  <si>
+    <t>:hh:`spine_top`</t>
+  </si>
+  <si>
+    <t>hex color string</t>
+  </si>
+  <si>
+    <t>enable primary x-axis range sharing across all subplots</t>
+  </si>
+  <si>
+    <t>enable primary y-axis range sharing across all subplots</t>
+  </si>
+  <si>
+    <t>enable primary z-axis range sharing across all subplots</t>
+  </si>
+  <si>
+    <t>enable secondary x-axis range sharing across all subplots</t>
+  </si>
+  <si>
+    <t>enable secondary y-axis range sharing across all subplots</t>
+  </si>
+  <si>
+    <t>enable axis range sharing for all subplots in a column of subplots</t>
+  </si>
+  <si>
+    <t>enable axis range sharing for all subplots in a row of subplots</t>
+  </si>
+  <si>
+    <t>show all axis edges</t>
+  </si>
+  <si>
+    <t>show bottom axis edge</t>
+  </si>
+  <si>
+    <t>show left axis edge</t>
+  </si>
+  <si>
+    <t>show right axis edge</t>
+  </si>
+  <si>
+    <t>show top axis edge</t>
+  </si>
+  <si>
+    <t>ticks_major_increment</t>
+  </si>
+  <si>
+    <t>ticks_&lt;major|minor&gt;_color</t>
+  </si>
+  <si>
+    <t>ticks_major_length</t>
+  </si>
+  <si>
+    <t>ticks_minor_length</t>
+  </si>
+  <si>
+    <t>ticks_major_width</t>
+  </si>
+  <si>
+    <t>ticks_minor_width</t>
+  </si>
+  <si>
+    <t>tick_minor_number</t>
+  </si>
+  <si>
+    <t>tick color</t>
+  </si>
+  <si>
+    <t>`Grids and ticks&lt;ticks.html#Increment&gt;`_</t>
+  </si>
+  <si>
+    <t>for major ticks only, the increment between tick marks</t>
+  </si>
+  <si>
+    <t>the length in pixels of the major tick lines</t>
+  </si>
+  <si>
+    <t>the length in pixels of the minor tick lines</t>
+  </si>
+  <si>
+    <t>thickness or edge width of a major tick mark</t>
+  </si>
+  <si>
+    <t>thickness or edge width of a minor tick mark</t>
+  </si>
+  <si>
+    <t>markers</t>
+  </si>
+  <si>
+    <t>boolean or list of str characters</t>
+  </si>
+  <si>
+    <t>if ``False``, turns off markers on the plot</t>
+  </si>
+  <si>
+    <t>if a list of characters, sets the markers to be used (one marker type per curve or data set)</t>
+  </si>
+  <si>
+    <t>default marker list</t>
+  </si>
+  <si>
+    <t>`Markers &lt;styles.html#Markers&gt;`_</t>
+  </si>
+  <si>
+    <t>marker_fill</t>
+  </si>
+  <si>
+    <t>turn on/off marker fill</t>
+  </si>
+  <si>
+    <t>marker_edge_color</t>
+  </si>
+  <si>
+    <t>marker_edge_width</t>
+  </si>
+  <si>
+    <t>marker_fill_color</t>
+  </si>
+  <si>
+    <t>marker_jitter</t>
+  </si>
+  <si>
+    <t>marker_size</t>
+  </si>
+  <si>
+    <t>set the marker edge color</t>
+  </si>
+  <si>
+    <t>match the line color scheme</t>
+  </si>
+  <si>
+    <t>set the marker edge width</t>
+  </si>
+  <si>
+    <t>set the marker fill color (only rendered if ``marker_fill=True``)</t>
+  </si>
+  <si>
+    <t>add a random offset or jitter to the points around their x-value (useful for box plots)</t>
+  </si>
+  <si>
+    <t>`True for boxplots | `False for all other plot types</t>
+  </si>
+  <si>
+    <t>hex color str</t>
+  </si>
+  <si>
+    <t>size of the markers (can be specified uniquely from the legend marker size)</t>
+  </si>
+  <si>
+    <t>`Marker size &lt;styles.html#Marker-size&gt;`_</t>
+  </si>
+  <si>
+    <t>polynomial degree for the fit</t>
+  </si>
+  <si>
+    <t>`Line fit &lt;plot.html#Line-fit&gt;`_</t>
+  </si>
+  <si>
+    <t>color of the fit line</t>
+  </si>
+  <si>
+    <t>display the fit equation on the plot</t>
+  </si>
+  <si>
+    <t>fit_color</t>
+  </si>
+  <si>
+    <t>fit_eqn</t>
+  </si>
+  <si>
+    <t>fit_font_size</t>
+  </si>
+  <si>
+    <t>fit_padding</t>
+  </si>
+  <si>
+    <t>fit_rsq</t>
+  </si>
+  <si>
+    <t>display the rsq of the fit on the plot</t>
+  </si>
+  <si>
+    <t>font size of the fit eqn and rsq value</t>
+  </si>
+  <si>
+    <t>padding in pixels from the top of the plot to the location of the fit eqn</t>
+  </si>
+  <si>
+    <t>:hh:`colors`</t>
+  </si>
+  <si>
+    <t>hex color str or list of hex color strs</t>
+  </si>
+  <si>
+    <t>colors to use for lines and markers</t>
+  </si>
+  <si>
+    <t>default list</t>
+  </si>
+  <si>
+    <t>`built-in color list &lt;styles.html#Built-in-color-list&gt;`_</t>
+  </si>
+  <si>
+    <t>:hh:`lines`</t>
+  </si>
+  <si>
+    <t>toggle line visibility</t>
   </si>
 </sst>
 </file>
@@ -516,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,6 +728,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,8 +1054,219 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EC7E2D-DCF8-4EF9-B918-01806BEF8232}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977791F3-80AC-4531-9CA4-7008D9DA2B1A}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4FEB52-878B-4D28-89A2-B1AB8C62A6E9}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,69 +1276,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" t="s">
-        <v>143</v>
+        <v>100</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" t="s">
-        <v>148</v>
+        <v>103</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +1332,95 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F6366-02F4-4896-860D-93253CEED381}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B32287C-42A7-457E-B4DB-9E939217B363}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -943,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -954,16 +1446,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,13 +1463,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -985,10 +1477,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>23</v>
@@ -996,27 +1488,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1043,10 +1535,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1059,268 +1551,268 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>55</v>
+      <c r="A2" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>56</v>
+      <c r="A4" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>57</v>
+      <c r="A7" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E9">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>62</v>
+      <c r="A12" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>63</v>
+      <c r="A16" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1340,17 +1832,20 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1364,10 +1859,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,13 +1870,13 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1391,17 +1886,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B8DBE5-887E-41ED-B9DC-6BC32D1444BD}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,7 +1906,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1423,278 +1920,348 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
         <v>74</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
-        <v>100</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
       <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>75</v>
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>99</v>
+        <v>155</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
       <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
+        <v>156</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E5:E9"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="D4:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1706,20 +2273,20 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1737,21 +2304,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23B93BB-8A29-4904-8DDB-E6FE296FB85A}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D896F12-1571-490A-B2C8-0EAA835668FE}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1764,23 +2338,120 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>144</v>
+      <c r="A2" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
+      <c r="A3" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>145</v>
+      <c r="A4" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4">
+        <v>6.2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>146</v>
+      <c r="A5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5">
+        <v>4.2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8">
+        <v>1.3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1789,28 +2460,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977791F3-80AC-4531-9CA4-7008D9DA2B1A}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4A1BF7-8BE4-4ABB-9BC6-B0D95AD85FDF}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1823,106 +2494,167 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
+      <c r="A2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>112</v>
+        <v>175</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>176</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>74</v>
+      <c r="A4" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>103</v>
+      <c r="A5" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>187</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>104</v>
+      <c r="A6" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>188</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>194</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E2:E6"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4FEB52-878B-4D28-89A2-B1AB8C62A6E9}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23B93BB-8A29-4904-8DDB-E6FE296FB85A}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1930,47 +2662,42 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>209</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="E2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
+        <v>213</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1979,24 +2706,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F6366-02F4-4896-860D-93253CEED381}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA3E29C-4580-4CDD-8302-895C0D68B708}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2004,61 +2735,110 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
+        <v>195</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
+        <v>197</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>105</v>
+        <v>198</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
axhline fix and doc update
</commit_message>
<xml_diff>
--- a/fivecentplots/doc/keywords.xlsx
+++ b/fivecentplots/doc/keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\fivecentplots\fivecentplots\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{26DAD7AC-DA79-4C8A-9E4E-7C208FFDF85B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0D79EBE1-CC8B-42C6-9A94-2E676235D7F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="671" firstSheet="3" activeTab="7" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="671" firstSheet="2" activeTab="2" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory" sheetId="11" r:id="rId1"/>
@@ -22,10 +22,13 @@
     <sheet name="Markers" sheetId="14" r:id="rId7"/>
     <sheet name="Lines" sheetId="4" r:id="rId8"/>
     <sheet name="Fit" sheetId="15" r:id="rId9"/>
-    <sheet name="Box" sheetId="7" r:id="rId10"/>
-    <sheet name="BoxDivider" sheetId="8" r:id="rId11"/>
-    <sheet name="BoxStat" sheetId="9" r:id="rId12"/>
-    <sheet name="BoxRange" sheetId="10" r:id="rId13"/>
+    <sheet name="Ref Line" sheetId="16" r:id="rId10"/>
+    <sheet name="Legend" sheetId="17" r:id="rId11"/>
+    <sheet name="Box" sheetId="7" r:id="rId12"/>
+    <sheet name="BoxDivider" sheetId="8" r:id="rId13"/>
+    <sheet name="BoxStat" sheetId="9" r:id="rId14"/>
+    <sheet name="BoxRange" sheetId="10" r:id="rId15"/>
+    <sheet name="WS" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="280">
   <si>
     <t>Keyword</t>
   </si>
@@ -51,9 +54,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>dpi</t>
-  </si>
-  <si>
     <t>fill_alpha</t>
   </si>
   <si>
@@ -267,15 +267,6 @@
     <t>other: ['symlog', 'logit']</t>
   </si>
   <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>size of the figure window</t>
-  </si>
-  <si>
-    <t>calculated automatically</t>
-  </si>
-  <si>
     <t>enable/disable a secondary y-axis (x-axis is "twinned" or duplicated across two y-axes)</t>
   </si>
   <si>
@@ -306,9 +297,6 @@
     <t>notch</t>
   </si>
   <si>
-    <t>zorder</t>
-  </si>
-  <si>
     <t>edge color of the boxes</t>
   </si>
   <si>
@@ -348,9 +336,6 @@
     <t>line color</t>
   </si>
   <si>
-    <t>relative z-height of line in plot</t>
-  </si>
-  <si>
     <t>box_stat_line_on</t>
   </si>
   <si>
@@ -372,9 +357,6 @@
     <t>toggle range lines on/off</t>
   </si>
   <si>
-    <t>style2</t>
-  </si>
-  <si>
     <t>#cccccc</t>
   </si>
   <si>
@@ -679,6 +661,225 @@
   </si>
   <si>
     <t>toggle line visibility</t>
+  </si>
+  <si>
+    <t>color of the reference line</t>
+  </si>
+  <si>
+    <t>`Reference line &lt;plot.html#Reference-line&gt;`_</t>
+  </si>
+  <si>
+    <t>legend text for the reference line</t>
+  </si>
+  <si>
+    <t>"Ref Line"</t>
+  </si>
+  <si>
+    <t>legend</t>
+  </si>
+  <si>
+    <t>name of a DataFrame column to use for grouping</t>
+  </si>
+  <si>
+    <t>`Legend &lt;plot.html#Legend&gt;`_</t>
+  </si>
+  <si>
+    <t>:hh:`location`</t>
+  </si>
+  <si>
+    <t>legend_marker_alpha</t>
+  </si>
+  <si>
+    <t>legend_marker_size</t>
+  </si>
+  <si>
+    <t>legend_points</t>
+  </si>
+  <si>
+    <t>legend_title</t>
+  </si>
+  <si>
+    <t>location of legend (at this time only outside of the plot is available!):</t>
+  </si>
+  <si>
+    <t>* 1 | "upper right" = upper right inside corner</t>
+  </si>
+  <si>
+    <t>* 2 | "upper left = upper left inside corner</t>
+  </si>
+  <si>
+    <t>* 0 | "outside" = outside of plot on right side</t>
+  </si>
+  <si>
+    <t>* 3 | "lower left" = lower left inside corner</t>
+  </si>
+  <si>
+    <t>int | str</t>
+  </si>
+  <si>
+    <t>* 4 | "lower right" = lower right inside corner</t>
+  </si>
+  <si>
+    <t>* 8 | "lower center"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 5 | "right" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 6 | "center left" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 7 | "center right" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 9 | "upper center" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 10 | "center" </t>
+  </si>
+  <si>
+    <t>alpha of the markers in the legend only</t>
+  </si>
+  <si>
+    <t>`Alpha &lt;styles.html#Alpha&gt;`_</t>
+  </si>
+  <si>
+    <t>marker size in legend only</t>
+  </si>
+  <si>
+    <t>same as ``marker_size``</t>
+  </si>
+  <si>
+    <t>number of points for each legend value</t>
+  </si>
+  <si>
+    <t>legend title text</t>
+  </si>
+  <si>
+    <t>defaults to legend column name</t>
+  </si>
+  <si>
+    <t>ws_label_col</t>
+  </si>
+  <si>
+    <t>ws_label_row</t>
+  </si>
+  <si>
+    <t>ws_col</t>
+  </si>
+  <si>
+    <t>ws_row</t>
+  </si>
+  <si>
+    <t>ws_fig_label</t>
+  </si>
+  <si>
+    <t>ws_leg_fig</t>
+  </si>
+  <si>
+    <t>ws_fig_ax</t>
+  </si>
+  <si>
+    <t>ws_label_tick</t>
+  </si>
+  <si>
+    <t>ws_leg_ax</t>
+  </si>
+  <si>
+    <t>ws_ticks_ax</t>
+  </si>
+  <si>
+    <t>ws_title_ax</t>
+  </si>
+  <si>
+    <t>ws_ax_fig</t>
+  </si>
+  <si>
+    <t>ws_tick_tick_minimum</t>
+  </si>
+  <si>
+    <t>ws_ax_box_title</t>
+  </si>
+  <si>
+    <t>Row/column grid</t>
+  </si>
+  <si>
+    <t>Figure</t>
+  </si>
+  <si>
+    <t>ws_fig_title</t>
+  </si>
+  <si>
+    <t>Axes</t>
+  </si>
+  <si>
+    <t>Ticks</t>
+  </si>
+  <si>
+    <t>Boxplot</t>
+  </si>
+  <si>
+    <t>col label to top edge of axes window</t>
+  </si>
+  <si>
+    <t>row label to right edge of axes window</t>
+  </si>
+  <si>
+    <t>space between columns</t>
+  </si>
+  <si>
+    <t>space between rows</t>
+  </si>
+  <si>
+    <t>left figure edge to ``label_y``</t>
+  </si>
+  <si>
+    <t>right legend edge to right figure edge</t>
+  </si>
+  <si>
+    <t>top figure edge to top of figure title</t>
+  </si>
+  <si>
+    <t>space between axis label and tick labels</t>
+  </si>
+  <si>
+    <t>right edge of axes to left edge of legend box</t>
+  </si>
+  <si>
+    <t>space between tick labels and axes</t>
+  </si>
+  <si>
+    <t>bottom edge of title to top edge of axes window</t>
+  </si>
+  <si>
+    <t>right edge of axes to right edge of figure with legend disabled</t>
+  </si>
+  <si>
+    <t>top figure edge to top edge of axes with figure title disabled</t>
+  </si>
+  <si>
+    <t>minimum space between consecutive ticks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right edge of axes to right edge of box title text </t>
+  </si>
+  <si>
+    <t>box_divider_color</t>
+  </si>
+  <si>
+    <t>box_range_lines_color</t>
+  </si>
+  <si>
+    <t>box_range_lines_style</t>
+  </si>
+  <si>
+    <t>box_range_lines_style2</t>
+  </si>
+  <si>
+    <t>box_stat_line_color</t>
+  </si>
+  <si>
+    <t>:hh:`dpi`</t>
   </si>
 </sst>
 </file>
@@ -714,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -732,11 +933,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,69 +1275,69 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
         <v>119</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
         <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1143,6 +1347,326 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060EFAE2-4230-4CC1-9B81-49FA07B9AEF2}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57959CA4-6648-4038-A65C-8F8FA5CA2A70}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D16" t="s">
+        <v>235</v>
+      </c>
+      <c r="E16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="B3:B14"/>
+    <mergeCell ref="D3:D14"/>
+    <mergeCell ref="E3:E14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977791F3-80AC-4531-9CA4-7008D9DA2B1A}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1164,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1178,80 +1702,80 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>96</v>
+        <v>32</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
       <c r="D3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
         <v>87</v>
       </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
       <c r="D5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
         <v>88</v>
       </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>93</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="E6" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1261,22 +1785,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4FEB52-878B-4D28-89A2-B1AB8C62A6E9}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1287,44 +1814,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1332,17 +1845,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F6366-02F4-4896-860D-93253CEED381}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="A11" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1361,58 +1874,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1420,22 +1919,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B32287C-42A7-457E-B4DB-9E939217B363}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1446,75 +1948,311 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>277</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>89</v>
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0532F2-0413-4C4B-B68D-AEF1E40DAF14}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
+        <v>243</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" t="s">
+        <v>266</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" t="s">
+        <v>268</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" t="s">
+        <v>270</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" t="s">
+        <v>272</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="C2:C16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1535,10 +2273,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1551,268 +2289,268 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>48</v>
+      <c r="A2" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
       </c>
       <c r="E9">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1829,10 +2567,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC55F79-79B3-4A74-88DE-7CAFD90BEB9A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1856,27 +2594,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1889,7 +2616,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1920,337 +2647,337 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>65</v>
+      <c r="B4" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2280,13 +3007,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2313,7 +3040,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -2321,11 +3048,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2338,120 +3065,120 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>160</v>
+      <c r="A2" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>159</v>
+      <c r="A3" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>161</v>
+      <c r="A4" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D4">
         <v>6.2</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>162</v>
+      <c r="A5" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D5">
         <v>4.2</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>165</v>
+      <c r="A6" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D7">
         <v>2.2000000000000002</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>164</v>
+      <c r="A8" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D8">
         <v>1.3</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2469,7 +3196,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -2477,11 +3204,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2494,131 +3221,131 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
         <v>181</v>
-      </c>
-      <c r="B5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" t="s">
-        <v>187</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>188</v>
       </c>
       <c r="D6">
         <v>1.5</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="B7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="D8" t="s">
         <v>184</v>
       </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D8" t="s">
-        <v>191</v>
-      </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>185</v>
+      <c r="A9" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2636,7 +3363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23B93BB-8A29-4904-8DDB-E6FE296FB85A}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2654,7 +3381,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2668,36 +3395,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2723,11 +3450,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2741,104 +3468,104 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>198</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>205</v>
       </c>
       <c r="D5">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>202</v>
+      <c r="A6" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
boxplot with varied x; doc updates
</commit_message>
<xml_diff>
--- a/fivecentplots/doc/keywords.xlsx
+++ b/fivecentplots/doc/keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\fivecentplots\fivecentplots\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0D79EBE1-CC8B-42C6-9A94-2E676235D7F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F21DC55F-28F4-4D3C-B682-8D0B0807E384}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="671" firstSheet="2" activeTab="2" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="862" firstSheet="9" activeTab="17" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory" sheetId="11" r:id="rId1"/>
@@ -29,6 +29,9 @@
     <sheet name="BoxStat" sheetId="9" r:id="rId14"/>
     <sheet name="BoxRange" sheetId="10" r:id="rId15"/>
     <sheet name="WS" sheetId="18" r:id="rId16"/>
+    <sheet name="Cbar" sheetId="19" r:id="rId17"/>
+    <sheet name="Contour" sheetId="21" r:id="rId18"/>
+    <sheet name="Heatmap" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="292">
   <si>
     <t>Keyword</t>
   </si>
@@ -880,6 +883,42 @@
   </si>
   <si>
     <t>:hh:`dpi`</t>
+  </si>
+  <si>
+    <t>toggle colorbar on/off for contour and heatmap plots</t>
+  </si>
+  <si>
+    <t>cbar width (height will match the height of the axes)</t>
+  </si>
+  <si>
+    <t>`contour example &lt;contour.html#Filled-contour&gt;`_</t>
+  </si>
+  <si>
+    <t>cmap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of a color map </t>
+  </si>
+  <si>
+    <t>inferno</t>
+  </si>
+  <si>
+    <t>:hh:`cbar`</t>
+  </si>
+  <si>
+    <t>:hh:`cmap`</t>
+  </si>
+  <si>
+    <t>:hh:`filled`</t>
+  </si>
+  <si>
+    <t>Fill area between contour lines</t>
+  </si>
+  <si>
+    <t>:hh:`levels`</t>
+  </si>
+  <si>
+    <t>Number of contour lines/levels to draw</t>
   </si>
 </sst>
 </file>
@@ -915,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -942,6 +981,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1350,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060EFAE2-4230-4CC1-9B81-49FA07B9AEF2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57959CA4-6648-4038-A65C-8F8FA5CA2A70}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,6 +2297,215 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB7194F-6935-4A3F-A6D1-D2440CFB36D0}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF9DEB0-6665-4538-AF49-F67F1AF6D966}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8856DC-C126-4FEE-B018-443AE2EE34DC}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA54C979-C4DA-4565-BB8F-88214FC12F78}">
   <dimension ref="A1:E18"/>
@@ -2569,7 +2818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC55F79-79B3-4A74-88DE-7CAFD90BEB9A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>